<commit_message>
Updated functional analysis for figure
</commit_message>
<xml_diff>
--- a/Stylophora_pistillata/differential_expression/results/kegg_res_padj0.05.xlsx
+++ b/Stylophora_pistillata/differential_expression/results/kegg_res_padj0.05.xlsx
@@ -576,22 +576,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0000921162907916414</v>
+        <v>0.0000921505047245825</v>
       </c>
       <c r="D2" t="n">
-        <v>3.80835350674964</v>
+        <v>3.80825536810288</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000921162907916414</v>
+        <v>0.0000921505047245827</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0170478364981966</v>
+        <v>0.0170444153530771</v>
       </c>
       <c r="G2" t="n">
         <v>144</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0000921162907916414</v>
+        <v>0.0000921505047245826</v>
       </c>
     </row>
     <row r="3">
@@ -602,22 +602,22 @@
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0000974162085611232</v>
+        <v>0.0000973966591604402</v>
       </c>
       <c r="D3" t="n">
-        <v>3.93486671683663</v>
+        <v>3.93492689321308</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0000974162085611234</v>
+        <v>0.0000973966591604405</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0170478364981966</v>
+        <v>0.0170444153530771</v>
       </c>
       <c r="G3" t="n">
         <v>57</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0000974162085611232</v>
+        <v>0.0000973966591604402</v>
       </c>
     </row>
     <row r="4">
@@ -628,22 +628,22 @@
         <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000245204030949148</v>
+        <v>0.000245306401787587</v>
       </c>
       <c r="D4" t="n">
-        <v>3.5051287829786</v>
+        <v>3.50501539230158</v>
       </c>
       <c r="E4" t="n">
-        <v>0.000245204030949148</v>
+        <v>0.000245306401787586</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0286071369440673</v>
+        <v>0.0286190802085517</v>
       </c>
       <c r="G4" t="n">
         <v>361</v>
       </c>
       <c r="H4" t="n">
-        <v>0.000245204030949149</v>
+        <v>0.000245306401787587</v>
       </c>
     </row>
   </sheetData>
@@ -694,22 +694,22 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0000101113509819203</v>
+        <v>0.0000101113509693054</v>
       </c>
       <c r="D2" t="n">
-        <v>4.35433264454316</v>
+        <v>4.35433264483962</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0000101113509819203</v>
+        <v>0.0000101113509693054</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0035389728436721</v>
+        <v>0.0035389728392569</v>
       </c>
       <c r="G2" t="n">
         <v>144</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0000101113509819203</v>
+        <v>0.0000101113509693054</v>
       </c>
     </row>
     <row r="3">
@@ -720,22 +720,22 @@
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0000624353888453495</v>
+        <v>0.0000624353887675353</v>
       </c>
       <c r="D3" t="n">
-        <v>3.85812108404797</v>
+        <v>3.85812108435923</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0000624353888453496</v>
+        <v>0.0000624353887675355</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00803647092466563</v>
+        <v>0.00803647092256032</v>
       </c>
       <c r="G3" t="n">
         <v>353</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0000624353888453495</v>
+        <v>0.0000624353887675354</v>
       </c>
     </row>
     <row r="4">
@@ -746,22 +746,22 @@
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>0.000111084372693519</v>
+        <v>0.000111084372641568</v>
       </c>
       <c r="D4" t="n">
-        <v>3.70995644899547</v>
+        <v>3.70995644911601</v>
       </c>
       <c r="E4" t="n">
-        <v>0.000111084372693519</v>
+        <v>0.000111084372641569</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00803647092466563</v>
+        <v>0.00803647092256032</v>
       </c>
       <c r="G4" t="n">
         <v>401</v>
       </c>
       <c r="H4" t="n">
-        <v>0.000111084372693519</v>
+        <v>0.000111084372641568</v>
       </c>
     </row>
     <row r="5">
@@ -772,22 +772,22 @@
         <v>19</v>
       </c>
       <c r="C5" t="n">
-        <v>0.000118452002953881</v>
+        <v>0.000118452002860247</v>
       </c>
       <c r="D5" t="n">
-        <v>3.72008644166049</v>
+        <v>3.72008644186968</v>
       </c>
       <c r="E5" t="n">
-        <v>0.000118452002953882</v>
+        <v>0.000118452002860247</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00803647092466563</v>
+        <v>0.00803647092256032</v>
       </c>
       <c r="G5" t="n">
         <v>168</v>
       </c>
       <c r="H5" t="n">
-        <v>0.000118452002953881</v>
+        <v>0.000118452002860247</v>
       </c>
     </row>
     <row r="6">
@@ -798,22 +798,22 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>0.000119414467459555</v>
+        <v>0.000119414467341135</v>
       </c>
       <c r="D6" t="n">
-        <v>3.72170828409165</v>
+        <v>3.7217082843546</v>
       </c>
       <c r="E6" t="n">
-        <v>0.000119414467459555</v>
+        <v>0.000119414467341135</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00803647092466563</v>
+        <v>0.00803647092256032</v>
       </c>
       <c r="G6" t="n">
         <v>159</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000119414467459555</v>
+        <v>0.000119414467341135</v>
       </c>
     </row>
     <row r="7">
@@ -824,22 +824,22 @@
         <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>0.000137768072994268</v>
+        <v>0.000137768072958177</v>
       </c>
       <c r="D7" t="n">
-        <v>3.81053628253279</v>
+        <v>3.81053628261327</v>
       </c>
       <c r="E7" t="n">
-        <v>0.000137768072994268</v>
+        <v>0.000137768072958177</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00803647092466563</v>
+        <v>0.00803647092256032</v>
       </c>
       <c r="G7" t="n">
         <v>57</v>
       </c>
       <c r="H7" t="n">
-        <v>0.000137768072994268</v>
+        <v>0.000137768072958177</v>
       </c>
     </row>
     <row r="8">
@@ -850,22 +850,22 @@
         <v>23</v>
       </c>
       <c r="C8" t="n">
-        <v>0.000170522770592935</v>
+        <v>0.000170522770430718</v>
       </c>
       <c r="D8" t="n">
-        <v>3.69253474724778</v>
+        <v>3.69253474752089</v>
       </c>
       <c r="E8" t="n">
-        <v>0.000170522770592935</v>
+        <v>0.000170522770430718</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00852613852964675</v>
+        <v>0.0085261385215359</v>
       </c>
       <c r="G8" t="n">
         <v>69</v>
       </c>
       <c r="H8" t="n">
-        <v>0.000170522770592935</v>
+        <v>0.000170522770430718</v>
       </c>
     </row>
     <row r="9">
@@ -876,22 +876,22 @@
         <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>0.000245800669746399</v>
+        <v>0.000245800669682784</v>
       </c>
       <c r="D9" t="n">
-        <v>3.52764080640167</v>
+        <v>3.52764080647329</v>
       </c>
       <c r="E9" t="n">
-        <v>0.000245800669746399</v>
+        <v>0.000245800669682783</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00985353734216556</v>
+        <v>0.00985353734201601</v>
       </c>
       <c r="G9" t="n">
         <v>155</v>
       </c>
       <c r="H9" t="n">
-        <v>0.000245800669746399</v>
+        <v>0.000245800669682784</v>
       </c>
     </row>
     <row r="10">
@@ -902,22 +902,22 @@
         <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>0.000284917603734819</v>
+        <v>0.000284917603700475</v>
       </c>
       <c r="D10" t="n">
-        <v>3.49149840743113</v>
+        <v>3.49149840746543</v>
       </c>
       <c r="E10" t="n">
-        <v>0.000284917603734818</v>
+        <v>0.000284917603700475</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00985353734216556</v>
+        <v>0.00985353734201601</v>
       </c>
       <c r="G10" t="n">
         <v>144</v>
       </c>
       <c r="H10" t="n">
-        <v>0.000284917603734819</v>
+        <v>0.000284917603700475</v>
       </c>
     </row>
     <row r="11">
@@ -928,22 +928,22 @@
         <v>13</v>
       </c>
       <c r="C11" t="n">
-        <v>0.000294312329779655</v>
+        <v>0.000294312329698809</v>
       </c>
       <c r="D11" t="n">
-        <v>3.45417919459067</v>
+        <v>3.45417919466619</v>
       </c>
       <c r="E11" t="n">
-        <v>0.000294312329779655</v>
+        <v>0.000294312329698808</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00985353734216556</v>
+        <v>0.00985353734201601</v>
       </c>
       <c r="G11" t="n">
         <v>361</v>
       </c>
       <c r="H11" t="n">
-        <v>0.000294312329779655</v>
+        <v>0.000294312329698809</v>
       </c>
     </row>
     <row r="12">
@@ -954,22 +954,22 @@
         <v>29</v>
       </c>
       <c r="C12" t="n">
-        <v>0.000309682602182346</v>
+        <v>0.000309682602177646</v>
       </c>
       <c r="D12" t="n">
-        <v>3.46870264102441</v>
+        <v>3.46870264102902</v>
       </c>
       <c r="E12" t="n">
-        <v>0.000309682602182346</v>
+        <v>0.000309682602177646</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00985353734216556</v>
+        <v>0.00985353734201601</v>
       </c>
       <c r="G12" t="n">
         <v>143</v>
       </c>
       <c r="H12" t="n">
-        <v>0.000309682602182346</v>
+        <v>0.000309682602177646</v>
       </c>
     </row>
     <row r="13">
@@ -980,22 +980,22 @@
         <v>31</v>
       </c>
       <c r="C13" t="n">
-        <v>0.000371651115718466</v>
+        <v>0.000371651115679445</v>
       </c>
       <c r="D13" t="n">
-        <v>3.39998791844683</v>
+        <v>3.39998791847615</v>
       </c>
       <c r="E13" t="n">
-        <v>0.000371651115718466</v>
+        <v>0.000371651115679445</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0108398242084553</v>
+        <v>0.0108398242073172</v>
       </c>
       <c r="G13" t="n">
         <v>206</v>
       </c>
       <c r="H13" t="n">
-        <v>0.000371651115718466</v>
+        <v>0.000371651115679445</v>
       </c>
     </row>
     <row r="14">
@@ -1006,22 +1006,22 @@
         <v>33</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00053633806705894</v>
+        <v>0.000536338066835952</v>
       </c>
       <c r="D14" t="n">
-        <v>3.31581784157684</v>
+        <v>3.31581784169752</v>
       </c>
       <c r="E14" t="n">
-        <v>0.00053633806705894</v>
+        <v>0.00053633806683595</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0144034880130679</v>
+        <v>0.0144034880096136</v>
       </c>
       <c r="G14" t="n">
         <v>118</v>
       </c>
       <c r="H14" t="n">
-        <v>0.00053633806705894</v>
+        <v>0.000536338066835952</v>
       </c>
     </row>
     <row r="15">
@@ -1032,22 +1032,22 @@
         <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>0.000600291065499562</v>
+        <v>0.000600291064899238</v>
       </c>
       <c r="D15" t="n">
-        <v>3.33993538643963</v>
+        <v>3.33993538675285</v>
       </c>
       <c r="E15" t="n">
-        <v>0.000600291065499562</v>
+        <v>0.000600291064899237</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0144034880130679</v>
+        <v>0.0144034880096136</v>
       </c>
       <c r="G15" t="n">
         <v>54</v>
       </c>
       <c r="H15" t="n">
-        <v>0.000600291065499562</v>
+        <v>0.000600291064899237</v>
       </c>
     </row>
     <row r="16">
@@ -1058,22 +1058,22 @@
         <v>37</v>
       </c>
       <c r="C16" t="n">
-        <v>0.000617292343417197</v>
+        <v>0.000617292343269154</v>
       </c>
       <c r="D16" t="n">
-        <v>3.26329317533487</v>
+        <v>3.26329317540505</v>
       </c>
       <c r="E16" t="n">
-        <v>0.000617292343417197</v>
+        <v>0.000617292343269154</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0144034880130679</v>
+        <v>0.0144034880096136</v>
       </c>
       <c r="G16" t="n">
         <v>145</v>
       </c>
       <c r="H16" t="n">
-        <v>0.000617292343417197</v>
+        <v>0.000617292343269154</v>
       </c>
     </row>
     <row r="17">
@@ -1084,22 +1084,22 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.000822446881299699</v>
+        <v>0.000822446880184488</v>
       </c>
       <c r="D17" t="n">
-        <v>3.17935465348886</v>
+        <v>3.17935465389609</v>
       </c>
       <c r="E17" t="n">
-        <v>0.000822446881299696</v>
+        <v>0.000822446880184488</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0171799217459694</v>
+        <v>0.0171799217438432</v>
       </c>
       <c r="G17" t="n">
         <v>151</v>
       </c>
       <c r="H17" t="n">
-        <v>0.000822446881299699</v>
+        <v>0.000822446880184488</v>
       </c>
     </row>
     <row r="18">
@@ -1110,22 +1110,22 @@
         <v>41</v>
       </c>
       <c r="C18" t="n">
-        <v>0.000834453341947086</v>
+        <v>0.000834453341843813</v>
       </c>
       <c r="D18" t="n">
-        <v>3.17971014314845</v>
+        <v>3.17971014318548</v>
       </c>
       <c r="E18" t="n">
-        <v>0.000834453341947084</v>
+        <v>0.000834453341843811</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0171799217459694</v>
+        <v>0.0171799217438432</v>
       </c>
       <c r="G18" t="n">
         <v>137</v>
       </c>
       <c r="H18" t="n">
-        <v>0.000834453341947086</v>
+        <v>0.000834453341843813</v>
       </c>
     </row>
     <row r="19">
@@ -1136,22 +1136,22 @@
         <v>43</v>
       </c>
       <c r="C19" t="n">
-        <v>0.00185992422462525</v>
+        <v>0.00185992422447794</v>
       </c>
       <c r="D19" t="n">
-        <v>2.91623830563264</v>
+        <v>2.91623830565784</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00185992422462524</v>
+        <v>0.00185992422447793</v>
       </c>
       <c r="F19" t="n">
-        <v>0.036165193256602</v>
+        <v>0.0361651932537376</v>
       </c>
       <c r="G19" t="n">
         <v>246</v>
       </c>
       <c r="H19" t="n">
-        <v>0.00185992422462524</v>
+        <v>0.00185992422447794</v>
       </c>
     </row>
     <row r="20">
@@ -1162,22 +1162,22 @@
         <v>45</v>
       </c>
       <c r="C20" t="n">
-        <v>0.00227894677365335</v>
+        <v>0.00227894677400765</v>
       </c>
       <c r="D20" t="n">
-        <v>2.88664324098758</v>
+        <v>2.88664324093343</v>
       </c>
       <c r="E20" t="n">
-        <v>0.00227894677365335</v>
+        <v>0.00227894677400766</v>
       </c>
       <c r="F20" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G20" t="n">
         <v>74</v>
       </c>
       <c r="H20" t="n">
-        <v>0.00227894677365335</v>
+        <v>0.00227894677400765</v>
       </c>
     </row>
     <row r="21">
@@ -1188,22 +1188,22 @@
         <v>47</v>
       </c>
       <c r="C21" t="n">
-        <v>0.00230764821555297</v>
+        <v>0.00230764821523644</v>
       </c>
       <c r="D21" t="n">
-        <v>2.84962453193788</v>
+        <v>2.84962453198253</v>
       </c>
       <c r="E21" t="n">
-        <v>0.00230764821555298</v>
+        <v>0.00230764821523645</v>
       </c>
       <c r="F21" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G21" t="n">
         <v>212</v>
       </c>
       <c r="H21" t="n">
-        <v>0.00230764821555298</v>
+        <v>0.00230764821523644</v>
       </c>
     </row>
     <row r="22">
@@ -1214,22 +1214,22 @@
         <v>49</v>
       </c>
       <c r="C22" t="n">
-        <v>0.00234038588980612</v>
+        <v>0.00234038588898522</v>
       </c>
       <c r="D22" t="n">
-        <v>3.23891642159857</v>
+        <v>3.23891642175393</v>
       </c>
       <c r="E22" t="n">
-        <v>0.00234038588980612</v>
+        <v>0.00234038588898522</v>
       </c>
       <c r="F22" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G22" t="n">
         <v>14</v>
       </c>
       <c r="H22" t="n">
-        <v>0.00234038588980612</v>
+        <v>0.00234038588898522</v>
       </c>
     </row>
     <row r="23">
@@ -1240,22 +1240,22 @@
         <v>51</v>
       </c>
       <c r="C23" t="n">
-        <v>0.00240718503447325</v>
+        <v>0.00240718503274619</v>
       </c>
       <c r="D23" t="n">
-        <v>2.8353996096697</v>
+        <v>2.83539960990356</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00240718503447325</v>
+        <v>0.0024071850327462</v>
       </c>
       <c r="F23" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G23" t="n">
         <v>200</v>
       </c>
       <c r="H23" t="n">
-        <v>0.00240718503447324</v>
+        <v>0.00240718503274619</v>
       </c>
     </row>
     <row r="24">
@@ -1266,22 +1266,22 @@
         <v>53</v>
       </c>
       <c r="C24" t="n">
-        <v>0.00246867069060341</v>
+        <v>0.00246867068944733</v>
       </c>
       <c r="D24" t="n">
-        <v>2.82735022358646</v>
+        <v>2.82735022373959</v>
       </c>
       <c r="E24" t="n">
-        <v>0.00246867069060341</v>
+        <v>0.00246867068944734</v>
       </c>
       <c r="F24" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G24" t="n">
         <v>209</v>
       </c>
       <c r="H24" t="n">
-        <v>0.00246867069060341</v>
+        <v>0.00246867068944733</v>
       </c>
     </row>
     <row r="25">
@@ -1292,22 +1292,22 @@
         <v>55</v>
       </c>
       <c r="C25" t="n">
-        <v>0.00259041981964134</v>
+        <v>0.00259041981775306</v>
       </c>
       <c r="D25" t="n">
-        <v>2.83869209392478</v>
+        <v>2.83869209417055</v>
       </c>
       <c r="E25" t="n">
-        <v>0.00259041981964134</v>
+        <v>0.00259041981775307</v>
       </c>
       <c r="F25" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G25" t="n">
         <v>77</v>
       </c>
       <c r="H25" t="n">
-        <v>0.00259041981964134</v>
+        <v>0.00259041981775306</v>
       </c>
     </row>
     <row r="26">
@@ -1318,22 +1318,22 @@
         <v>57</v>
       </c>
       <c r="C26" t="n">
-        <v>0.00265492113288107</v>
+        <v>0.00265492113124127</v>
       </c>
       <c r="D26" t="n">
-        <v>2.82288441830277</v>
+        <v>2.82288441850865</v>
       </c>
       <c r="E26" t="n">
-        <v>0.00265492113288107</v>
+        <v>0.00265492113124128</v>
       </c>
       <c r="F26" t="n">
-        <v>0.037168895860335</v>
+        <v>0.0371688958373779</v>
       </c>
       <c r="G26" t="n">
         <v>95</v>
       </c>
       <c r="H26" t="n">
-        <v>0.00265492113288107</v>
+        <v>0.00265492113124127</v>
       </c>
     </row>
     <row r="27">
@@ -1344,22 +1344,22 @@
         <v>59</v>
       </c>
       <c r="C27" t="n">
-        <v>0.00303301487377407</v>
+        <v>0.0030330148724712</v>
       </c>
       <c r="D27" t="n">
-        <v>2.77059648740494</v>
+        <v>2.77059648754932</v>
       </c>
       <c r="E27" t="n">
-        <v>0.00303301487377408</v>
+        <v>0.00303301487247121</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0395206078253382</v>
+        <v>0.0395206078094212</v>
       </c>
       <c r="G27" t="n">
         <v>115</v>
       </c>
       <c r="H27" t="n">
-        <v>0.00303301487377407</v>
+        <v>0.0030330148724712</v>
       </c>
     </row>
     <row r="28">
@@ -1370,22 +1370,22 @@
         <v>61</v>
       </c>
       <c r="C28" t="n">
-        <v>0.00304873260366894</v>
+        <v>0.00304873260244106</v>
       </c>
       <c r="D28" t="n">
-        <v>2.7595880188505</v>
+        <v>2.75958801898482</v>
       </c>
       <c r="E28" t="n">
-        <v>0.00304873260366895</v>
+        <v>0.00304873260244106</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0395206078253382</v>
+        <v>0.0395206078094212</v>
       </c>
       <c r="G28" t="n">
         <v>178</v>
       </c>
       <c r="H28" t="n">
-        <v>0.00304873260366894</v>
+        <v>0.00304873260244106</v>
       </c>
     </row>
     <row r="29">
@@ -1396,22 +1396,22 @@
         <v>63</v>
       </c>
       <c r="C29" t="n">
-        <v>0.00329282726155789</v>
+        <v>0.00329282726006794</v>
       </c>
       <c r="D29" t="n">
-        <v>2.73216368859196</v>
+        <v>2.73216368874411</v>
       </c>
       <c r="E29" t="n">
-        <v>0.00329282726155789</v>
+        <v>0.00329282726006794</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0411603407694737</v>
+        <v>0.0411603407508493</v>
       </c>
       <c r="G29" t="n">
         <v>201</v>
       </c>
       <c r="H29" t="n">
-        <v>0.00329282726155789</v>
+        <v>0.00329282726006794</v>
       </c>
     </row>
     <row r="30">
@@ -1422,22 +1422,22 @@
         <v>65</v>
       </c>
       <c r="C30" t="n">
-        <v>0.00384156090912929</v>
+        <v>0.00384156090578075</v>
       </c>
       <c r="D30" t="n">
-        <v>2.68701555824472</v>
+        <v>2.68701555854414</v>
       </c>
       <c r="E30" t="n">
-        <v>0.00384156090912929</v>
+        <v>0.00384156090578075</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0463636661446639</v>
+        <v>0.0463636661042504</v>
       </c>
       <c r="G30" t="n">
         <v>134</v>
       </c>
       <c r="H30" t="n">
-        <v>0.00384156090912929</v>
+        <v>0.00384156090578075</v>
       </c>
     </row>
   </sheetData>

</xml_diff>